<commit_message>
Include Remove and View_models
</commit_message>
<xml_diff>
--- a/Log/calibration_log.xlsx
+++ b/Log/calibration_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0346E7-41BD-324C-8A84-D622F7D7E959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBDCEC5-F295-1C4A-B1FA-84D87E604F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{70EFF65A-D3A6-CC4B-ADFE-BB01482CA67A}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,10 @@
     <t>Count</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>E50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +187,12 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +216,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -224,6 +234,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,31 +453,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>11</c:v>
@@ -476,46 +489,46 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>6</c:v>
@@ -2560,10 +2573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3910397-879A-B340-99A2-0ECA78893F04}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -3474,6 +3487,65 @@
       <c r="Q17" s="1">
         <v>1400</v>
       </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="4">
+        <v>44594</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1">
+        <v>100</v>
+      </c>
+      <c r="E18" s="1">
+        <v>200</v>
+      </c>
+      <c r="F18" s="1">
+        <v>300</v>
+      </c>
+      <c r="G18" s="1">
+        <v>400</v>
+      </c>
+      <c r="H18" s="1">
+        <v>450</v>
+      </c>
+      <c r="I18" s="1">
+        <v>650</v>
+      </c>
+      <c r="J18" s="1">
+        <v>700</v>
+      </c>
+      <c r="K18" s="1">
+        <v>800</v>
+      </c>
+      <c r="L18" s="1">
+        <v>900</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1050</v>
+      </c>
+      <c r="O18" s="1">
+        <v>1100</v>
+      </c>
+      <c r="P18" s="1">
+        <v>1200</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="C21" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q29" xr:uid="{B3910397-879A-B340-99A2-0ECA78893F04}">
@@ -4408,7 +4480,7 @@
       </c>
       <c r="B26" s="1" cm="1">
         <f t="array" ref="B26">SUM(COUNTIF(A26,'High DA'!$C$2:$Q$58))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5">
         <v>5</v>
@@ -4424,7 +4496,7 @@
       </c>
       <c r="B27" s="1" cm="1">
         <f t="array" ref="B27">SUM(COUNTIF(A27,'High DA'!$C$2:$Q$58))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27" s="5">
         <v>10</v>
@@ -4456,7 +4528,7 @@
       </c>
       <c r="B29" s="1" cm="1">
         <f t="array" ref="B29">SUM(COUNTIF(A29,'High DA'!$C$2:$Q$58))</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" s="5">
         <v>20</v>
@@ -4488,7 +4560,7 @@
       </c>
       <c r="B31" s="1" cm="1">
         <f t="array" ref="B31">SUM(COUNTIF(A31,'High DA'!$C$2:$Q$58))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D31" s="5">
         <v>30</v>
@@ -4520,7 +4592,7 @@
       </c>
       <c r="B33" s="1" cm="1">
         <f t="array" ref="B33">SUM(COUNTIF(A33,'High DA'!$C$2:$Q$58))</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" s="5">
         <v>40</v>
@@ -4536,7 +4608,7 @@
       </c>
       <c r="B34" s="1" cm="1">
         <f t="array" ref="B34">SUM(COUNTIF(A34,'High DA'!$C$2:$Q$58))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5">
         <v>45</v>
@@ -4600,7 +4672,7 @@
       </c>
       <c r="B38" s="1" cm="1">
         <f t="array" ref="B38">SUM(COUNTIF(A38,'High DA'!$C$2:$Q$58))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D38" s="5">
         <v>65</v>
@@ -4616,7 +4688,7 @@
       </c>
       <c r="B39" s="1" cm="1">
         <f t="array" ref="B39">SUM(COUNTIF(A39,'High DA'!$C$2:$Q$58))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39" s="5">
         <v>70</v>
@@ -4648,7 +4720,7 @@
       </c>
       <c r="B41" s="1" cm="1">
         <f t="array" ref="B41">SUM(COUNTIF(A41,'High DA'!$C$2:$Q$58))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="5">
         <v>80</v>
@@ -4680,7 +4752,7 @@
       </c>
       <c r="B43" s="1" cm="1">
         <f t="array" ref="B43">SUM(COUNTIF(A43,'High DA'!$C$2:$Q$58))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43" s="5">
         <v>90</v>
@@ -4712,7 +4784,7 @@
       </c>
       <c r="B45" s="1" cm="1">
         <f t="array" ref="B45">SUM(COUNTIF(A45,'High DA'!$C$2:$Q$58))</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D45" s="5">
         <v>100</v>
@@ -4728,7 +4800,7 @@
       </c>
       <c r="B46" s="1" cm="1">
         <f t="array" ref="B46">SUM(COUNTIF(A46,'High DA'!$C$2:$Q$58))</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" s="5">
         <v>105</v>
@@ -4744,7 +4816,7 @@
       </c>
       <c r="B47" s="1" cm="1">
         <f t="array" ref="B47">SUM(COUNTIF(A47,'High DA'!$C$2:$Q$58))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47" s="5">
         <v>110</v>
@@ -4776,7 +4848,7 @@
       </c>
       <c r="B49" s="1" cm="1">
         <f t="array" ref="B49">SUM(COUNTIF(A49,'High DA'!$C$2:$Q$58))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D49" s="5">
         <v>120</v>
@@ -4808,7 +4880,7 @@
       </c>
       <c r="B51" s="1" cm="1">
         <f t="array" ref="B51">SUM(COUNTIF(A51,'High DA'!$C$2:$Q$58))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D51" s="5">
         <v>130</v>

</xml_diff>

<commit_message>
Include clustering before EN model
</commit_message>
<xml_diff>
--- a/Log/calibration_log.xlsx
+++ b/Log/calibration_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/Log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBDCEC5-F295-1C4A-B1FA-84D87E604F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60F56A9-CABB-C04A-8E5E-B6B7CBFB347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{70EFF65A-D3A6-CC4B-ADFE-BB01482CA67A}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,6 +138,9 @@
   <si>
     <t>E50</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E50</t>
   </si>
 </sst>
 </file>
@@ -915,7 +918,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -927,28 +930,28 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>9</c:v>
@@ -969,19 +972,19 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>6</c:v>
@@ -993,16 +996,16 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3560,7 +3563,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52D6D4A-A531-C440-8D8C-AFEB17EECC6F}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
@@ -4208,6 +4211,59 @@
         <v>130</v>
       </c>
       <c r="Q12" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="4">
+        <v>44599</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>55</v>
+      </c>
+      <c r="I13" s="1">
+        <v>60</v>
+      </c>
+      <c r="J13" s="1">
+        <v>95</v>
+      </c>
+      <c r="K13" s="1">
+        <v>100</v>
+      </c>
+      <c r="L13" s="1">
+        <v>110</v>
+      </c>
+      <c r="M13" s="1">
+        <v>115</v>
+      </c>
+      <c r="N13" s="1">
+        <v>135</v>
+      </c>
+      <c r="O13" s="1">
+        <v>140</v>
+      </c>
+      <c r="P13" s="1">
+        <v>145</v>
+      </c>
+      <c r="Q13" s="1">
         <v>150</v>
       </c>
     </row>
@@ -4487,7 +4543,7 @@
       </c>
       <c r="E26" s="1" cm="1">
         <f t="array" ref="E26">SUM(COUNTIF(D26,'Low DA'!$C$2:$Q$60))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4551,7 +4607,7 @@
       </c>
       <c r="E30" s="1" cm="1">
         <f t="array" ref="E30">SUM(COUNTIF(D30,'Low DA'!$C$2:$Q$60))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4583,7 +4639,7 @@
       </c>
       <c r="E32" s="1" cm="1">
         <f t="array" ref="E32">SUM(COUNTIF(D32,'Low DA'!$C$2:$Q$60))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4615,7 +4671,7 @@
       </c>
       <c r="E34" s="1" cm="1">
         <f t="array" ref="E34">SUM(COUNTIF(D34,'Low DA'!$C$2:$Q$60))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4631,7 +4687,7 @@
       </c>
       <c r="E35" s="1" cm="1">
         <f t="array" ref="E35">SUM(COUNTIF(D35,'Low DA'!$C$2:$Q$60))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -4647,7 +4703,7 @@
       </c>
       <c r="E36" s="1" cm="1">
         <f t="array" ref="E36">SUM(COUNTIF(D36,'Low DA'!$C$2:$Q$60))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -4663,7 +4719,7 @@
       </c>
       <c r="E37" s="1" cm="1">
         <f t="array" ref="E37">SUM(COUNTIF(D37,'Low DA'!$C$2:$Q$60))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -4775,7 +4831,7 @@
       </c>
       <c r="E44" s="1" cm="1">
         <f t="array" ref="E44">SUM(COUNTIF(D44,'Low DA'!$C$2:$Q$60))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -4791,7 +4847,7 @@
       </c>
       <c r="E45" s="1" cm="1">
         <f t="array" ref="E45">SUM(COUNTIF(D45,'Low DA'!$C$2:$Q$60))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -4823,7 +4879,7 @@
       </c>
       <c r="E47" s="1" cm="1">
         <f t="array" ref="E47">SUM(COUNTIF(D47,'Low DA'!$C$2:$Q$60))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -4839,7 +4895,7 @@
       </c>
       <c r="E48" s="1" cm="1">
         <f t="array" ref="E48">SUM(COUNTIF(D48,'Low DA'!$C$2:$Q$60))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4903,7 +4959,7 @@
       </c>
       <c r="E52" s="1" cm="1">
         <f t="array" ref="E52">SUM(COUNTIF(D52,'Low DA'!$C$2:$Q$60))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -4919,7 +4975,7 @@
       </c>
       <c r="E53" s="1" cm="1">
         <f t="array" ref="E53">SUM(COUNTIF(D53,'Low DA'!$C$2:$Q$60))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -4935,7 +4991,7 @@
       </c>
       <c r="E54" s="1" cm="1">
         <f t="array" ref="E54">SUM(COUNTIF(D54,'Low DA'!$C$2:$Q$60))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4951,7 +5007,7 @@
       </c>
       <c r="E55" s="1" cm="1">
         <f t="array" ref="E55">SUM(COUNTIF(D55,'Low DA'!$C$2:$Q$60))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ElasticNet and Octaflow_preprocess
</commit_message>
<xml_diff>
--- a/Log/calibration_log.xlsx
+++ b/Log/calibration_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/Script/Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60F56A9-CABB-C04A-8E5E-B6B7CBFB347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4151441B-EC00-EF48-9F93-72D7DED5376E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{70EFF65A-D3A6-CC4B-ADFE-BB01482CA67A}"/>
   </bookViews>
@@ -140,7 +140,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>E50</t>
+    <t>E59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2579,7 +2580,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -3566,7 +3567,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -4060,7 +4061,7 @@
         <v>44529</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -4216,7 +4217,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="4">
-        <v>44599</v>
+        <v>44602</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>

</xml_diff>